<commit_message>
Major update to AFOLU, including revisions to LRAF, SOC accounting, demands and exports, and fake_data_complete.csv
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/AFOLU/ipcc_afolu_c2_general_use_tables.xlsx
+++ b/ref/data_tables_and_derivations/AFOLU/ipcc_afolu_c2_general_use_tables.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ipcc_data_tables_and_derivations/AFOLU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/AFOLU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A11D68-F608-2846-8501-94046181E6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796FA253-72A6-6A4E-8CD1-A664B754FD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24220" windowHeight="17520" xr2:uid="{0F7B3AC4-6872-894F-9C5F-CA57A58590FF}"/>
+    <workbookView xWindow="4600" yWindow="460" windowWidth="24220" windowHeight="17520" activeTab="1" xr2:uid="{0F7B3AC4-6872-894F-9C5F-CA57A58590FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2.3" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 5.5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>climate region</t>
   </si>
   <si>
-    <t>boreal</t>
-  </si>
-  <si>
     <t>cold temperate, dry</t>
   </si>
   <si>
@@ -116,6 +114,54 @@
   </si>
   <si>
     <t>KT N2O CO2E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>LU Fctors</t>
+  </si>
+  <si>
+    <t>FLU</t>
+  </si>
+  <si>
+    <t>Long Term Cultivated</t>
+  </si>
+  <si>
+    <t>Cool Temperate/Boreal</t>
+  </si>
+  <si>
+    <t>Warm Temperate</t>
+  </si>
+  <si>
+    <t>Tropical</t>
+  </si>
+  <si>
+    <t>moist</t>
+  </si>
+  <si>
+    <t>moist/wet</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>temperate/boreal</t>
+  </si>
+  <si>
+    <t>perennial</t>
+  </si>
+  <si>
+    <t>mean lu factor</t>
+  </si>
+  <si>
+    <t>FMG</t>
+  </si>
+  <si>
+    <t>Reduced Till</t>
+  </si>
+  <si>
+    <t>No Till</t>
   </si>
 </sst>
 </file>
@@ -489,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2309310-36C2-3042-96FD-24727249267F}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,30 +549,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="2">
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -540,7 +586,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
@@ -552,7 +598,7 @@
         <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1">
         <v>20</v>
@@ -560,7 +606,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>95</v>
@@ -580,7 +626,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>38</v>
@@ -592,7 +638,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1">
         <v>70</v>
@@ -600,7 +646,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>88</v>
@@ -612,7 +658,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1">
         <v>80</v>
@@ -620,7 +666,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>38</v>
@@ -632,7 +678,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>50</v>
@@ -640,7 +686,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>65</v>
@@ -652,7 +698,7 @@
         <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1">
         <v>70</v>
@@ -660,7 +706,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>44</v>
@@ -672,7 +718,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1">
         <v>130</v>
@@ -680,7 +726,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>88</v>
@@ -692,7 +738,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1">
         <v>80</v>
@@ -700,7 +746,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <f>AVERAGE(B3:F3,B5:F5,B7:F7)</f>
@@ -723,12 +769,16 @@
         <v>1.9004524886877827</v>
       </c>
       <c r="G12">
-        <v>36.833333333333336</v>
+        <v>36.8333333333333</v>
+      </c>
+      <c r="I12">
+        <f>(G12+G13)/2</f>
+        <v>56.122549019607824</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <f>AVERAGE(B4:F4,B6:F6,B8:F8,B9:F9)</f>
@@ -756,7 +806,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <f>AVERAGE(B7:F10)</f>
@@ -785,12 +835,12 @@
         <v>100</v>
       </c>
       <c r="K14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <f>AVERAGE(B2:B6,E4,F2:F6)</f>
@@ -819,12 +869,12 @@
         <v>10</v>
       </c>
       <c r="K15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <f>AVERAGE(C2:D6)</f>
@@ -854,16 +904,15 @@
         <v>5.4999999999999993E-2</v>
       </c>
       <c r="K16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <f>AVERAGE(B2:F6)</f>
-        <v>60.19047619047619</v>
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
       </c>
       <c r="C17">
         <f>MIN(B2:F6)</f>
@@ -873,31 +922,35 @@
         <f>MAX(B2:F6)</f>
         <v>130</v>
       </c>
-      <c r="E17">
-        <f t="shared" ref="E17" si="2">C17/B17</f>
-        <v>0.16613924050632911</v>
-      </c>
-      <c r="F17">
-        <f t="shared" ref="F17" si="3">D17/B17</f>
-        <v>2.1598101265822787</v>
+      <c r="E17" t="e">
+        <f>C17/B17</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" t="e">
+        <f t="shared" ref="F17" si="2">D17/B17</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G17">
-        <v>60.19047619047619</v>
+        <v>60.190476190476197</v>
+      </c>
+      <c r="I17">
+        <f>(G15+G16+G14)/3</f>
+        <v>56.852693602693599</v>
       </c>
       <c r="J17">
         <f>J16*(11/7)*310</f>
         <v>26.792857142857137</v>
       </c>
       <c r="K17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E19">
-        <v>0.51583710407239813</v>
+        <v>0.51583710407239802</v>
       </c>
       <c r="F19">
         <v>1.9004524886877827</v>
@@ -959,6 +1012,254 @@
       </c>
       <c r="G24">
         <v>60.19047619047619</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885D8C39-4C7F-3B41-8378-12A73BEC09B5}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>0.72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>1.01</v>
+      </c>
+      <c r="F10">
+        <f>AVERAGE(E2:E10)</f>
+        <v>0.79999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17">
+        <v>1.04</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(E12:E17)</f>
+        <v>1.0149999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F24">
+        <f>AVERAGE(E19:E24)</f>
+        <v>1.0666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with import export data
</commit_message>
<xml_diff>
--- a/ref/data_tables_and_derivations/AFOLU/ipcc_afolu_c2_general_use_tables.xlsx
+++ b/ref/data_tables_and_derivations/AFOLU/ipcc_afolu_c2_general_use_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/data_tables_and_derivations/AFOLU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796FA253-72A6-6A4E-8CD1-A664B754FD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD2C5D6-CAD5-F54A-819A-5DF34AE64998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="460" windowWidth="24220" windowHeight="17520" activeTab="1" xr2:uid="{0F7B3AC4-6872-894F-9C5F-CA57A58590FF}"/>
+    <workbookView xWindow="8720" yWindow="460" windowWidth="24220" windowHeight="17520" activeTab="1" xr2:uid="{0F7B3AC4-6872-894F-9C5F-CA57A58590FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2.3" sheetId="1" r:id="rId1"/>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>